<commit_message>
se agrega procolo y pines al informe
</commit_message>
<xml_diff>
--- a/Informe-Final/diagramas/pines utilizados.xlsx
+++ b/Informe-Final/diagramas/pines utilizados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\magicbox\Informe-Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\magicbox\Informe-Final\diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116BD48A-6328-4B3C-BEF9-E18C188EA867}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854DF123-FD94-4ABE-AE0A-8B11EC409DA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CC6D668-1D3F-4CAA-9BA5-75885B032887}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>PINES UTILIZADOS</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>7, 8</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Coolers 1 y 2</t>
   </si>
 </sst>
 </file>
@@ -164,16 +176,16 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3C80C3-6E3E-46D9-9E8B-4CC650DA3FE7}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,136 +516,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>12</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>